<commit_message>
Added K Means Demo
</commit_message>
<xml_diff>
--- a/SalesOpportunityDataSet.xlsx
+++ b/SalesOpportunityDataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\Documents\SourceCode\DATA_SCIENCE\ai_and_data_repo_0001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{638AA5ED-1235-4FF9-97ED-4202E67186AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21D846D-FEA3-4A9F-874C-160FFF5AC5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3165" windowWidth="17865" windowHeight="9615" xr2:uid="{C5225A0F-519C-4735-9BAC-D4BAFAFFF564}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="19725" windowHeight="11385" xr2:uid="{C5225A0F-519C-4735-9BAC-D4BAFAFFF564}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOpportunityDataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
   <si>
     <t>Opportunity_ID</t>
   </si>
@@ -185,6 +185,21 @@
   </si>
   <si>
     <t>Clinical Director</t>
+  </si>
+  <si>
+    <t>Operations Director</t>
+  </si>
+  <si>
+    <t>Technology Specialist</t>
+  </si>
+  <si>
+    <t>Cybersecurity Officer</t>
+  </si>
+  <si>
+    <t>Director of FinOps</t>
+  </si>
+  <si>
+    <t>E-commerce Manager</t>
   </si>
 </sst>
 </file>
@@ -668,8 +683,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69F66D5-9795-4E81-81BB-30AD94844590}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,6 +1733,166 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1021</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="1">
+        <v>92</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1022</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1">
+        <v>51</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="1">
+        <v>9</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1023</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="1">
+        <v>70</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="1">
+        <v>6</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="1">
+        <v>85</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1025</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="1">
+        <v>45</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>